<commit_message>
Paper Research addition and final changes
</commit_message>
<xml_diff>
--- a/Experiments (Azam Maam).xlsx
+++ b/Experiments (Azam Maam).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamza\Machine Learning Assignments\NSGA-2-for-Feature-Selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17B7729-45AC-403F-BFE7-02A3D248D2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55081D52-C52A-4655-BF25-0AC28A6CE77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{451468FA-B28D-4634-B037-730E472A4561}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="66">
   <si>
     <t>Dataset</t>
   </si>
@@ -126,13 +126,131 @@
   </si>
   <si>
     <t>Sixth Set(MIC) +0.2</t>
+  </si>
+  <si>
+    <t>Wilcoxon Rank Sum Test</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>P-value: 0.13057001811573618.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.023342202012890823.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.00015705228423075119.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.002496908915141548.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.4496917979688909.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.16197241048012612.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 1.0.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.7623688184698398.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.5453496680111236.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.08209870865427452.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.04125001659393949.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison Between Set 2 and Set 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison Between Set 2 and Set 6 </t>
+  </si>
+  <si>
+    <t>P-value: 0.01910992220684444.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison Between Set 4 and Set 5 </t>
+  </si>
+  <si>
+    <t>P-value: 0.1124105846553637.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.06964240479832813.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.06402210128302689.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.08897301170181328.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.04936619475193269.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.40567889528505297.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.12122450301291662.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.49629170223109287.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.0031970994479345307.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.028365505605209992.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison Between Set 4 and Set 6 </t>
+  </si>
+  <si>
+    <t>P-value: 0.00579535854433471.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.0005828399431792743.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.00021218287122257815.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.6501474440948545.The two sets of numbers are not significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.0019397281129030408.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.00038105845205068544.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <t>P-value: 0.008150971593502691.The two sets of numbers are significantly different.</t>
+  </si>
+  <si>
+    <r>
+      <t>import</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inherit"/>
+      </rPr>
+      <t xml:space="preserve"> os</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +283,43 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF303F9F"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -278,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -307,10 +462,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -320,6 +471,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,6 +514,65 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D124-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>103</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>2369820</xdr:colOff>
+          <xdr:row>107</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Control 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -653,32 +891,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BDA8F0-2B89-414F-A3BA-DCC5210B80EB}">
-  <dimension ref="A1:J101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BDA8F0-2B89-414F-A3BA-DCC5210B80EB}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:M105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="5" max="5" width="19.5546875" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="70.109375" customWidth="1"/>
     <col min="8" max="8" width="19.77734375" customWidth="1"/>
     <col min="9" max="9" width="20.21875" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="22.109375" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="21">
       <c r="A1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F1" s="30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,20 +933,23 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.6">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -711,23 +959,29 @@
       <c r="C3" s="4">
         <v>0.32631578900000002</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -737,23 +991,29 @@
       <c r="C4" s="5">
         <v>8.7096774000000002E-2</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="5">
         <v>0.26721272800000001</v>
       </c>
-      <c r="H4" s="18">
+      <c r="K4" s="5">
         <v>0.294736842</v>
       </c>
-      <c r="I4" s="5">
+      <c r="L4" s="5">
         <v>0.23683999999999999</v>
       </c>
-      <c r="J4" s="14">
+      <c r="M4" s="14">
         <v>0.20523</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -763,23 +1023,29 @@
       <c r="C5" s="5">
         <v>9.0909090999999997E-2</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="5">
         <v>7.7546403999999999E-2</v>
       </c>
-      <c r="H5" s="18">
+      <c r="K5" s="5">
         <v>9.6774193999999994E-2</v>
       </c>
-      <c r="I5" s="5">
+      <c r="L5" s="5">
         <v>5.806E-2</v>
       </c>
-      <c r="J5" s="14">
+      <c r="M5" s="14">
         <v>3.8710000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -789,23 +1055,29 @@
       <c r="C6" s="5">
         <v>0.25172413799999999</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="5">
         <v>0.13453358300000001</v>
       </c>
-      <c r="H6" s="18">
+      <c r="K6" s="5">
         <v>0.16818181800000001</v>
       </c>
-      <c r="I6" s="5">
+      <c r="L6" s="5">
         <v>5.9089999999999997E-2</v>
       </c>
-      <c r="J6" s="14">
+      <c r="M6" s="14">
         <v>9.0900000000000009E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -815,23 +1087,29 @@
       <c r="C7" s="5">
         <v>0.37272727300000003</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="5">
         <v>0.29978339199999998</v>
       </c>
-      <c r="H7" s="18">
+      <c r="K7" s="5">
         <v>0.20344827600000001</v>
       </c>
-      <c r="I7" s="5">
+      <c r="L7" s="5">
         <v>0.14828</v>
       </c>
-      <c r="J7" s="14">
+      <c r="M7" s="14">
         <v>9.3100000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -841,23 +1119,29 @@
       <c r="C8" s="5">
         <v>0.23076923099999999</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="5">
         <v>0.263549696</v>
       </c>
-      <c r="H8" s="18">
+      <c r="K8" s="5">
         <v>0.19545454500000001</v>
       </c>
-      <c r="I8" s="5">
+      <c r="L8" s="5">
         <v>0.30454999999999999</v>
       </c>
-      <c r="J8" s="14">
+      <c r="M8" s="14">
         <v>1.3639999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -867,23 +1151,29 @@
       <c r="C9" s="5">
         <v>0.10491803299999999</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="5">
         <v>0.237888552</v>
       </c>
-      <c r="H9" s="14">
+      <c r="K9" s="14">
         <v>0.22307692300000001</v>
       </c>
-      <c r="I9" s="5">
+      <c r="L9" s="5">
         <v>0.24359</v>
       </c>
-      <c r="J9" s="5">
+      <c r="M9" s="5">
         <v>0.22650000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -893,23 +1183,29 @@
       <c r="C10" s="5">
         <v>0.4</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="5">
         <v>0.10227731</v>
       </c>
-      <c r="H10" s="18">
+      <c r="K10" s="5">
         <v>0.10491803299999999</v>
       </c>
-      <c r="I10" s="5">
+      <c r="L10" s="5">
         <v>8.8520000000000001E-2</v>
       </c>
-      <c r="J10" s="14">
+      <c r="M10" s="14">
         <v>7.5410000000000005E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -919,23 +1215,29 @@
       <c r="C11" s="5">
         <v>0.48823529399999999</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="5">
         <v>0.346200801</v>
       </c>
-      <c r="H11" s="18">
+      <c r="K11" s="5">
         <v>0.32666666700000002</v>
       </c>
-      <c r="I11" s="5">
+      <c r="L11" s="5">
         <v>0.38</v>
       </c>
-      <c r="J11" s="14">
+      <c r="M11" s="14">
         <v>0.18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
@@ -945,23 +1247,29 @@
       <c r="C12" s="5">
         <v>0.37413793099999998</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="5">
         <v>0.44137544400000001</v>
       </c>
-      <c r="H12" s="18">
+      <c r="K12" s="5">
         <v>0.37058823499999999</v>
       </c>
-      <c r="I12" s="5">
+      <c r="L12" s="5">
         <v>0.45294000000000001</v>
       </c>
-      <c r="J12" s="14">
+      <c r="M12" s="14">
         <v>0.36176000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
@@ -971,23 +1279,29 @@
       <c r="C13" s="5">
         <v>0.10370370399999999</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="5">
         <v>0.32029981400000002</v>
       </c>
-      <c r="H13" s="14">
+      <c r="K13" s="14">
         <v>0.243103448</v>
       </c>
-      <c r="I13" s="5">
+      <c r="L13" s="5">
         <v>0.46034000000000003</v>
       </c>
-      <c r="J13" s="5">
+      <c r="M13" s="5">
         <v>0.35861999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -997,23 +1311,29 @@
       <c r="C14" s="5">
         <v>0.28448275899999997</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="5">
         <v>0.114743522</v>
       </c>
-      <c r="H14" s="18">
+      <c r="K14" s="5">
         <v>0.12592592599999999</v>
       </c>
-      <c r="I14" s="5">
+      <c r="L14" s="5">
         <v>0.11481</v>
       </c>
-      <c r="J14" s="14">
+      <c r="M14" s="14">
         <v>3.7039999999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -1023,23 +1343,29 @@
       <c r="C15" s="5">
         <v>0.31333333299999999</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="5">
         <v>0.23648909600000001</v>
       </c>
-      <c r="H15" s="14">
+      <c r="K15" s="14">
         <v>0.205172414</v>
       </c>
-      <c r="I15" s="5">
+      <c r="L15" s="5">
         <v>0.33276</v>
       </c>
-      <c r="J15" s="5">
+      <c r="M15" s="5">
         <v>0.27413999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -1049,350 +1375,457 @@
       <c r="C16" s="7">
         <v>0.368421053</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="5">
         <v>0.33601141200000001</v>
       </c>
-      <c r="H16" s="18">
+      <c r="K16" s="5">
         <v>0.34333333300000002</v>
       </c>
-      <c r="I16" s="5">
+      <c r="L16" s="5">
         <v>0.40476000000000001</v>
       </c>
-      <c r="J16" s="5">
+      <c r="M16" s="5">
         <v>0.38889000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F17" s="6" t="s">
+    <row r="17" spans="1:13">
+      <c r="F17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="7">
         <v>0.37775803099999999</v>
       </c>
-      <c r="H17" s="19">
+      <c r="K17" s="7">
         <v>0.41578947399999999</v>
       </c>
-      <c r="I17" s="7">
+      <c r="L17" s="7">
         <v>0.33333000000000002</v>
       </c>
-      <c r="J17" s="15">
+      <c r="M17" s="15">
         <v>0.33333000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="15.6">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="J19" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="K19" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="L19" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="15.6">
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="5">
         <v>0.26721272800000001</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="20">
+      <c r="J20" s="3">
         <v>5.9</v>
       </c>
-      <c r="H20" s="9">
+      <c r="K20" s="9">
         <v>6.8</v>
       </c>
-      <c r="I20" s="22">
+      <c r="L20" s="18">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="5">
         <v>7.7546403999999999E-2</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="20">
+      <c r="J21" s="3">
         <v>19.170000000000002</v>
       </c>
-      <c r="H21" s="9">
+      <c r="K21" s="9">
         <v>3.3</v>
       </c>
-      <c r="I21" s="22">
+      <c r="L21" s="18">
         <v>4.3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="5">
         <v>0.13453358300000001</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="20">
+      <c r="J22" s="3">
         <v>3.97</v>
       </c>
-      <c r="H22" s="9">
+      <c r="K22" s="9">
         <v>3.2</v>
       </c>
-      <c r="I22" s="22">
+      <c r="L22" s="18">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="5">
         <v>0.29978339199999998</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="20">
+      <c r="J23" s="3">
         <v>10.99</v>
       </c>
-      <c r="H23" s="9">
+      <c r="K23" s="9">
         <v>37.9</v>
       </c>
-      <c r="I23" s="22">
+      <c r="L23" s="18">
         <v>73.099999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="5">
         <v>0.263549696</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="20">
+      <c r="J24" s="3">
         <v>20.79</v>
       </c>
-      <c r="H24" s="9">
+      <c r="K24" s="9">
         <v>1.7</v>
       </c>
-      <c r="I24" s="22">
+      <c r="L24" s="18">
         <v>5.9</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13">
       <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="5">
         <v>0.237888552</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="20">
+      <c r="J25" s="3">
         <v>107.14</v>
       </c>
-      <c r="H25" s="9">
+      <c r="K25" s="9">
         <v>3.11</v>
       </c>
-      <c r="I25" s="22">
+      <c r="L25" s="18">
         <v>3.33</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13">
       <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="5">
         <v>0.10227731</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="20">
+      <c r="J26" s="3">
         <v>6.5</v>
       </c>
-      <c r="H26" s="9">
+      <c r="K26" s="9">
         <v>19.899999999999999</v>
       </c>
-      <c r="I26" s="22">
+      <c r="L26" s="18">
         <v>45.6</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="5">
         <v>0.346200801</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="20">
+      <c r="J27" s="3">
         <v>20.420000000000002</v>
       </c>
-      <c r="H27" s="9">
+      <c r="K27" s="9">
         <v>26.4</v>
       </c>
-      <c r="I27" s="22">
+      <c r="L27" s="18">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="5">
         <v>0.44137544400000001</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="20">
+      <c r="J28" s="3">
         <v>60.42</v>
       </c>
-      <c r="H28" s="9">
+      <c r="K28" s="9">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I28" s="22">
+      <c r="L28" s="18">
         <v>10.1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13">
       <c r="A29" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="5">
         <v>0.32029981400000002</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="20">
+      <c r="J29" s="3">
         <v>80.89</v>
       </c>
-      <c r="H29" s="9">
+      <c r="K29" s="9">
         <v>29.5</v>
       </c>
-      <c r="I29" s="22">
+      <c r="L29" s="18">
         <v>51.5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13">
       <c r="A30" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B30" s="5">
         <v>0.114743522</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G30" s="20">
+      <c r="J30" s="3">
         <v>5.78</v>
       </c>
-      <c r="H30" s="9">
+      <c r="K30" s="9">
         <v>4.5</v>
       </c>
-      <c r="I30" s="22">
+      <c r="L30" s="18">
         <v>23.7</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B31" s="5">
         <v>0.23648909600000001</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="20">
+      <c r="J31" s="3">
         <v>176.04</v>
       </c>
-      <c r="H31" s="9">
+      <c r="K31" s="9">
         <v>30.4</v>
       </c>
-      <c r="I31" s="22">
+      <c r="L31" s="18">
         <v>48.6</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="5">
         <v>0.33601141200000001</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="20">
+      <c r="J32" s="3">
         <v>1331.54</v>
       </c>
-      <c r="H32" s="9">
+      <c r="K32" s="9">
         <v>2.2799999999999998</v>
       </c>
-      <c r="I32" s="22">
+      <c r="L32" s="18">
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B33" s="7">
         <v>0.37775803099999999</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="21">
+      <c r="J33" s="6">
         <v>73.73</v>
       </c>
-      <c r="H33" s="10">
+      <c r="K33" s="10">
         <v>2.67</v>
       </c>
-      <c r="I33" s="23">
+      <c r="L33" s="19">
         <v>2.67</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
+      <c r="F34" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="15.6">
       <c r="A36" s="8" t="s">
         <v>0</v>
       </c>
@@ -1402,8 +1835,11 @@
       <c r="C36" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.6">
       <c r="A37" s="5" t="s">
         <v>3</v>
       </c>
@@ -1413,8 +1849,14 @@
       <c r="C37" s="5">
         <v>0.25789473699999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F37" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="5" t="s">
         <v>4</v>
       </c>
@@ -1424,8 +1866,14 @@
       <c r="C38" s="5">
         <v>5.4838709999999999E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F38" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
@@ -1435,8 +1883,14 @@
       <c r="C39" s="5">
         <v>7.2727279000000006E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="5" t="s">
         <v>6</v>
       </c>
@@ -1446,8 +1900,14 @@
       <c r="C40" s="5">
         <v>0.14827586200000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="5" t="s">
         <v>7</v>
       </c>
@@ -1457,8 +1917,14 @@
       <c r="C41" s="5">
         <v>0.29090909100000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="5" t="s">
         <v>8</v>
       </c>
@@ -1468,8 +1934,14 @@
       <c r="C42" s="5">
         <v>0.29230769200000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="5" t="s">
         <v>9</v>
       </c>
@@ -1479,8 +1951,14 @@
       <c r="C43" s="5">
         <v>9.0163934000000001E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="5" t="s">
         <v>10</v>
       </c>
@@ -1490,8 +1968,14 @@
       <c r="C44" s="5">
         <v>0.34666666699999998</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" s="5" t="s">
         <v>11</v>
       </c>
@@ -1501,8 +1985,14 @@
       <c r="C45" s="5">
         <v>0.39117647100000003</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F45" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="5" t="s">
         <v>12</v>
       </c>
@@ -1512,8 +2002,14 @@
       <c r="C46" s="5">
         <v>0.36724137899999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="5" t="s">
         <v>13</v>
       </c>
@@ -1523,8 +2019,14 @@
       <c r="C47" s="5">
         <v>0.114814815</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" s="5" t="s">
         <v>14</v>
       </c>
@@ -1534,8 +2036,14 @@
       <c r="C48" s="5">
         <v>0.31896551699999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="5" t="s">
         <v>15</v>
       </c>
@@ -1545,8 +2053,14 @@
       <c r="C49" s="5">
         <v>0.41333333300000002</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F49" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="7" t="s">
         <v>16</v>
       </c>
@@ -1556,138 +2070,247 @@
       <c r="C50" s="7">
         <v>0.321052632</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="F51" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="15.6">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.6">
       <c r="A54" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B54" s="5">
         <v>0.294736842</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F54" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="5">
         <v>9.6774193999999994E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F55" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B56" s="5">
         <v>0.16818181800000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F56" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="5">
         <v>0.20344827600000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F57" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B58" s="5">
         <v>0.19545454500000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B59" s="5">
         <v>0.22307692300000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F59" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B60" s="5">
         <v>0.10491803299999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B61" s="5">
         <v>0.32666666700000002</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B62" s="5">
         <v>0.37058823499999999</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G62" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B63" s="5">
         <v>0.243103448</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F63" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G63" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B64" s="5">
         <v>0.12592592599999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B65" s="5">
         <v>0.205172414</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B66" s="5">
         <v>0.34333333300000002</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F66" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G66" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B67" s="7">
         <v>0.41578947399999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="F68" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="15.6">
       <c r="A70" s="8" t="s">
         <v>0</v>
       </c>
@@ -1698,7 +2321,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7">
       <c r="A71" s="5" t="s">
         <v>3</v>
       </c>
@@ -1709,7 +2332,7 @@
         <v>0.23683999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7">
       <c r="A72" s="5" t="s">
         <v>4</v>
       </c>
@@ -1720,7 +2343,7 @@
         <v>5.806E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7">
       <c r="A73" s="5" t="s">
         <v>5</v>
       </c>
@@ -1731,7 +2354,7 @@
         <v>5.9089999999999997E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7">
       <c r="A74" s="5" t="s">
         <v>6</v>
       </c>
@@ -1742,7 +2365,7 @@
         <v>0.14828</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7">
       <c r="A75" s="5" t="s">
         <v>7</v>
       </c>
@@ -1753,7 +2376,7 @@
         <v>0.30454999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7">
       <c r="A76" s="5" t="s">
         <v>8</v>
       </c>
@@ -1764,7 +2387,7 @@
         <v>0.24359</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7">
       <c r="A77" s="5" t="s">
         <v>9</v>
       </c>
@@ -1775,7 +2398,7 @@
         <v>8.8520000000000001E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7">
       <c r="A78" s="5" t="s">
         <v>10</v>
       </c>
@@ -1786,7 +2409,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7">
       <c r="A79" s="5" t="s">
         <v>11</v>
       </c>
@@ -1797,7 +2420,7 @@
         <v>0.45294000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7">
       <c r="A80" s="5" t="s">
         <v>12</v>
       </c>
@@ -1808,7 +2431,7 @@
         <v>0.46034000000000003</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3">
       <c r="A81" s="5" t="s">
         <v>13</v>
       </c>
@@ -1819,7 +2442,7 @@
         <v>0.11481</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3">
       <c r="A82" s="5" t="s">
         <v>14</v>
       </c>
@@ -1830,7 +2453,7 @@
         <v>0.33276</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3">
       <c r="A83" s="5" t="s">
         <v>15</v>
       </c>
@@ -1841,7 +2464,7 @@
         <v>0.40476000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3">
       <c r="A84" s="7" t="s">
         <v>16</v>
       </c>
@@ -1852,12 +2475,12 @@
         <v>0.33333000000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="15.6">
       <c r="A87" s="8" t="s">
         <v>0</v>
       </c>
@@ -1868,7 +2491,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3">
       <c r="A88" s="5" t="s">
         <v>3</v>
       </c>
@@ -1879,7 +2502,7 @@
         <v>0.20523</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3">
       <c r="A89" s="5" t="s">
         <v>4</v>
       </c>
@@ -1890,7 +2513,7 @@
         <v>3.8710000000000001E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3">
       <c r="A90" s="5" t="s">
         <v>5</v>
       </c>
@@ -1901,7 +2524,7 @@
         <v>9.0900000000000009E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3">
       <c r="A91" s="5" t="s">
         <v>6</v>
       </c>
@@ -1912,7 +2535,7 @@
         <v>9.3100000000000002E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3">
       <c r="A92" s="5" t="s">
         <v>7</v>
       </c>
@@ -1923,7 +2546,7 @@
         <v>1.3639999999999999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3">
       <c r="A93" s="5" t="s">
         <v>8</v>
       </c>
@@ -1934,7 +2557,7 @@
         <v>0.22650000000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3">
       <c r="A94" s="5" t="s">
         <v>9</v>
       </c>
@@ -1945,7 +2568,7 @@
         <v>7.5410000000000005E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3">
       <c r="A95" s="5" t="s">
         <v>10</v>
       </c>
@@ -1956,7 +2579,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3">
       <c r="A96" s="5" t="s">
         <v>11</v>
       </c>
@@ -1967,7 +2590,7 @@
         <v>0.36176000000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7">
       <c r="A97" s="5" t="s">
         <v>12</v>
       </c>
@@ -1978,7 +2601,7 @@
         <v>0.35861999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7">
       <c r="A98" s="5" t="s">
         <v>13</v>
       </c>
@@ -1989,7 +2612,7 @@
         <v>3.7039999999999997E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7">
       <c r="A99" s="5" t="s">
         <v>14</v>
       </c>
@@ -2000,7 +2623,7 @@
         <v>0.27413999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7">
       <c r="A100" s="5" t="s">
         <v>15</v>
       </c>
@@ -2011,7 +2634,7 @@
         <v>0.38889000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7">
       <c r="A101" s="7" t="s">
         <v>16</v>
       </c>
@@ -2022,7 +2645,47 @@
         <v>0.33333000000000002</v>
       </c>
     </row>
+    <row r="103" spans="1:7">
+      <c r="G103" s="26"/>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="G104" s="27"/>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="G105" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId3" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>103</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>2369820</xdr:colOff>
+                <xdr:row>107</xdr:row>
+                <xdr:rowOff>22860</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId3" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
</xml_diff>